<commit_message>
bugfix: corrigido geração de código na planilha
</commit_message>
<xml_diff>
--- a/api-files-maker.xlsx
+++ b/api-files-maker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DevProjects\project-templates\template-api-ts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B506F22-9459-4C40-8FE2-33D9B893931F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2F8373-6A1D-40EB-9B4E-4DB9BD28AFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{75994CF3-CE13-42EB-B49D-C2778692B7AF}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="39">
   <si>
     <t>fora do constructor</t>
   </si>
@@ -809,45 +809,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -869,6 +830,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1212,12 +1212,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
       <c r="H1" s="47"/>
       <c r="I1" s="48" t="s">
         <v>38</v>
@@ -1229,10 +1229,10 @@
         <f>LOWER(I1)&amp;"s"</f>
         <v>stores</v>
       </c>
-      <c r="P1" s="65" t="s">
+      <c r="P1" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="66"/>
+      <c r="Q1" s="77"/>
     </row>
     <row r="2" spans="2:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1"/>
@@ -1242,8 +1242,8 @@
       <c r="L2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="68"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="79"/>
       <c r="W2" s="39"/>
     </row>
     <row r="3" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1251,15 +1251,15 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="I3" s="60" t="s">
+      <c r="I3" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="61"/>
-      <c r="K3" s="62"/>
-      <c r="P3" s="58" t="s">
+      <c r="J3" s="72"/>
+      <c r="K3" s="73"/>
+      <c r="P3" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="Q3" s="59"/>
+      <c r="Q3" s="70"/>
       <c r="U3" s="43"/>
       <c r="V3" s="43"/>
       <c r="W3" s="43"/>
@@ -1296,10 +1296,10 @@
       <c r="M4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="56" t="s">
+      <c r="P4" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" s="57"/>
+      <c r="Q4" s="68"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="U4" s="44"/>
@@ -1607,11 +1607,11 @@
       <c r="AE16" s="40"/>
     </row>
     <row r="17" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I17" s="60" t="s">
+      <c r="I17" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="J17" s="61"/>
-      <c r="K17" s="62"/>
+      <c r="J17" s="72"/>
+      <c r="K17" s="73"/>
       <c r="L17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="AE17" s="40"/>
@@ -2082,7 +2082,7 @@
   <dimension ref="B1:AC39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+      <selection activeCell="AD18" sqref="AD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2855,8 +2855,9 @@
         <f>IF(Entry!P6="x","public set created(date: Date) {this._created = date; }","")</f>
         <v>public set created(date: Date) {this._created = date; }</v>
       </c>
-      <c r="F13" t="s">
-        <v>18</v>
+      <c r="F13" t="str">
+        <f>IF(Entry!D16="x",Entry!J16&amp;": this._"&amp;Entry!J16&amp;", ","")</f>
+        <v/>
       </c>
       <c r="H13" s="54"/>
       <c r="M13" s="54"/>
@@ -2888,8 +2889,9 @@
         <f>IF(Entry!Q6="x","public set updated(date: Date) {this._updated = date; }","")</f>
         <v>public set updated(date: Date) {this._updated = date; }</v>
       </c>
-      <c r="F14" t="s">
-        <v>18</v>
+      <c r="F14" t="str">
+        <f>IF(Entry!D17="x",Entry!J17&amp;": this._"&amp;Entry!J17&amp;", ","")</f>
+        <v/>
       </c>
       <c r="H14" s="54"/>
       <c r="M14" s="54"/>
@@ -2925,8 +2927,9 @@
         <f>E2&amp;E3&amp;E4&amp;E5&amp;E6&amp;E7&amp;E8&amp;E9&amp;E10&amp;E11&amp;E12&amp;E13&amp;E14</f>
         <v>public set id(id: string) { this._id = id; }public set created(date: Date) {this._created = date; }public set updated(date: Date) {this._updated = date; }</v>
       </c>
-      <c r="F15" t="s">
-        <v>18</v>
+      <c r="F15" t="str">
+        <f>IF(Entry!D18="x",Entry!J18&amp;": this._"&amp;Entry!J18&amp;", ","")</f>
+        <v/>
       </c>
       <c r="H15" s="54"/>
       <c r="J15" t="str">
@@ -3014,8 +3017,9 @@
         <f>IF(Entry!F19="x","public set "&amp;Entry!J19&amp;"("&amp;Entry!J19&amp;": "&amp;Entry!K19&amp;") { this._"&amp;Entry!J19&amp;" = "&amp;Entry!J19&amp;"; }","")</f>
         <v>public set name(name: string) { this._name = name; }</v>
       </c>
-      <c r="F18" t="s">
-        <v>18</v>
+      <c r="F18" t="str">
+        <f>IF(Entry!D19="x",Entry!J19&amp;": this._"&amp;Entry!J19&amp;", ","")</f>
+        <v xml:space="preserve">name: this._name, </v>
       </c>
       <c r="G18" t="str">
         <f>IF(Entry!B19=1,"entity."&amp;Entry!J19&amp;", ","")</f>
@@ -3068,8 +3072,9 @@
         <f>IF(Entry!F20="x","public set "&amp;Entry!J20&amp;"("&amp;Entry!J20&amp;": "&amp;Entry!K20&amp;") { this._"&amp;Entry!J20&amp;" = "&amp;Entry!J20&amp;"; }","")</f>
         <v>public set price(price: number) { this._price = price; }</v>
       </c>
-      <c r="F19" t="s">
-        <v>18</v>
+      <c r="F19" t="str">
+        <f>IF(Entry!D20="x",Entry!J20&amp;": this._"&amp;Entry!J20&amp;", ","")</f>
+        <v xml:space="preserve">price: this._price, </v>
       </c>
       <c r="G19" t="str">
         <f>IF(Entry!B20=1,"entity."&amp;Entry!J20&amp;", ","")</f>
@@ -3825,7 +3830,7 @@
       </c>
       <c r="F37" t="str">
         <f>F2&amp;F3&amp;F4&amp;F5&amp;F6&amp;F7&amp;F8&amp;F9&amp;F10&amp;F11&amp;F12&amp;F18&amp;F19&amp;F20&amp;F21&amp;F22&amp;F23&amp;F24&amp;F25&amp;F26&amp;F27&amp;F28&amp;F29&amp;F30&amp;F31&amp;F32&amp;F33&amp;F34&amp;F35&amp;F36</f>
-        <v xml:space="preserve">id: this._id,   </v>
+        <v xml:space="preserve">id: this._id, name: this._name, price: this._price, </v>
       </c>
       <c r="G37" t="str">
         <f>G18&amp;G19&amp;G20&amp;G21&amp;G22&amp;G23&amp;G24&amp;G25&amp;G26&amp;G27&amp;G28&amp;G29&amp;G30&amp;G31&amp;G32&amp;G33&amp;G34&amp;G35&amp;G36</f>
@@ -3848,7 +3853,7 @@
     <row r="38" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F38" t="str">
         <f>"public toJson() { return { "&amp;F37&amp;" }; }"</f>
-        <v>public toJson() { return { id: this._id,    }; }</v>
+        <v>public toJson() { return { id: this._id, name: this._name, price: this._price,  }; }</v>
       </c>
       <c r="G38" t="str">
         <f>"public static "&amp;G17&amp;"(entity: any) { const created = new "&amp;Entry!I1&amp;"("&amp;Engine!G37&amp;"); created.id = entity.id; return created; }"</f>
@@ -3884,9 +3889,6 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="F37" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -3895,7 +3897,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3907,108 +3909,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="74"/>
-      <c r="B1" s="75"/>
+      <c r="A1" s="61"/>
+      <c r="B1" s="62"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="71"/>
+      <c r="B2" s="58"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="str">
+      <c r="A3" s="57" t="str">
         <f>Engine!G1&amp;"export class "&amp;Entry!I1&amp;" {"&amp;Engine!B15&amp;" constructor("&amp;Engine!B37&amp;") {"&amp;Engine!C15&amp;Engine!C37&amp;"}"&amp;Engine!D15&amp;Engine!D37&amp;Engine!E15&amp;Engine!E37&amp;Engine!F38&amp;Engine!G38&amp;"}"</f>
-        <v>import { v4 as createUuid } from 'uuid';export class Store {private _id: string; private _created?: Date;private _updated?: Date; constructor(private _name: string, private _price: number, ) {this._id = createUuid(); this._name = _name; this._price = _price; }public get id(): string {return this._id; } public get created(): Date {return this._created!; }public get updated(): Date {return this._updated!; }public get name(): string {return this._name; } public get price(): number {return this._price; } public set id(id: string) { this._id = id; }public set created(date: Date) {this._created = date; }public set updated(date: Date) {this._updated = date; }public set name(name: string) { this._name = name; }public set price(price: number) { this._price = price; }public toJson() { return { id: this._id,    }; }public static create(entity: any) { const created = new Store(entity.name, entity.price, ); created.id = entity.id; return created; }}</v>
-      </c>
-      <c r="B3" s="72" t="str">
+        <v>import { v4 as createUuid } from 'uuid';export class Store {private _id: string; private _created?: Date;private _updated?: Date; constructor(private _name: string, private _price: number, ) {this._id = createUuid(); this._name = _name; this._price = _price; }public get id(): string {return this._id; } public get created(): Date {return this._created!; }public get updated(): Date {return this._updated!; }public get name(): string {return this._name; } public get price(): number {return this._price; } public set id(id: string) { this._id = id; }public set created(date: Date) {this._created = date; }public set updated(date: Date) {this._updated = date; }public set name(name: string) { this._name = name; }public set price(price: number) { this._price = price; }public toJson() { return { id: this._id, name: this._name, price: this._price,  }; }public static create(entity: any) { const created = new Store(entity.name, entity.price, ); created.id = entity.id; return created; }}</v>
+      </c>
+      <c r="B3" s="59" t="str">
         <f>"&lt;-- Colar dentro de um arquivo .ts - nome sugerido: "&amp;LOWER(Entry!$I$1)&amp;".model.ts"</f>
         <v>&lt;-- Colar dentro de um arquivo .ts - nome sugerido: store.model.ts</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="76"/>
-      <c r="B4" s="77"/>
+      <c r="A4" s="63"/>
+      <c r="B4" s="64"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="73"/>
+      <c r="B5" s="60"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="70" t="str">
+      <c r="A6" s="57" t="str">
         <f>Engine!L15&amp;"@Entity('"&amp;Entry!K1&amp;"') export class "&amp;Entry!I1&amp;"Entity {"&amp;Engine!J15&amp;Engine!J37&amp;"} // Relacionamentos precisam ser configurados"</f>
         <v>import { Entity, Column, PrimaryColumn, CreateDateColumn, UpdateDateColumn } from 'typeorm'; @Entity('stores') export class StoreEntity {@PrimaryColumn()id: string; @Column()name: string; @Column()price: number; @CreateDateColumn() created: Date;@UpdateDateColumn() updated: Date;} // Relacionamentos precisam ser configurados</v>
       </c>
-      <c r="B6" s="72" t="str">
+      <c r="B6" s="59" t="str">
         <f>"&lt;-- Colar dentro de um arquivo .ts - nome sugerido: "&amp;LOWER(Entry!$I$1)&amp;".entity.ts"</f>
         <v>&lt;-- Colar dentro de um arquivo .ts - nome sugerido: store.entity.ts</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="76"/>
-      <c r="B7" s="77"/>
+      <c r="A7" s="63"/>
+      <c r="B7" s="64"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="73"/>
+      <c r="B8" s="60"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="70" t="str">
+      <c r="A9" s="57" t="str">
         <f>Engine!P1&amp;Engine!P2&amp;"export class "&amp;Entry!I1&amp;Engine!N1&amp;" { "&amp;Engine!Q1&amp;Engine!R1&amp;" }"&amp;Engine!Q2&amp;Engine!R2&amp;" }"&amp;Engine!Q3&amp;Engine!R3&amp;" }"&amp;Engine!Q4&amp;Engine!R4&amp;" }"&amp;Engine!Q5&amp;Engine!R5&amp;" }"&amp;" } // Configurar os usecases corretos e imports"</f>
         <v>import { Request, Response } from 'express'; import { ApiResponse } from '../../../shared/util/http-response.adapter'; export class StoreController { public async create(req: Request, res: Response) {try { const { name,price, } = req.body; const result = await new methodUseCase().execute({ name,price, }); return ApiResponse.done(res, result); } catch (error: any) { return ApiResponse.serverError(res, error); } }public async list(req: Request, res: Response) {try { const result = await new methodUseCase().execute(); return ApiResponse.done(res, result); } catch (error: any) { return ApiResponse.serverError(res, error); } }public async get(req: Request, res: Response) {try { const { id } = req.params; const result = await new methodUseCase().execute(id); return ApiResponse.done(res, result); } catch (error: any) { return ApiResponse.serverError(res, error); } }public async update(req: Request, res: Response) {try { const { id } = req.params; const { name,price, } = req.body; const result = await new methodUseCase().execute({ name,price, }); return ApiResponse.done(res, result); } catch (error: any) { return ApiResponse.serverError(res, error); } }public async delete(req: Request, res: Response) {try { const { id } = req.params; const result = await new methodUseCase().execute(id); return ApiResponse.done(res, result); } catch (error: any) { return ApiResponse.serverError(res, error); } } } // Configurar os usecases corretos e imports</v>
       </c>
-      <c r="B9" s="72" t="str">
+      <c r="B9" s="59" t="str">
         <f>"&lt;-- Colar dentro de um arquivo .ts - nome sugerido: "&amp;LOWER(Entry!$I$1)&amp;".controller.ts"</f>
         <v>&lt;-- Colar dentro de um arquivo .ts - nome sugerido: store.controller.ts</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="76"/>
-      <c r="B10" s="77"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="64"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="73"/>
+      <c r="B11" s="60"/>
     </row>
     <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="70" t="str">
+      <c r="A12" s="57" t="str">
         <f>Engine!V1&amp;" export class "&amp;Entry!I1&amp;Engine!T1&amp;" { "&amp;Engine!W2&amp;Engine!W3&amp;Engine!W4&amp;Engine!W5&amp;Engine!W6&amp;Engine!W7&amp;Engine!W8&amp;" } //Corrigir imports e adicionar outros métodos de acordo com o projeto"</f>
         <v>import { Database } from '../../../../main/database/database.connection'; export class StoreRepository { private connection = Database.connection.getRepository(StoreEntity);public async create(store: Store) { const storeEntity = this.connection.create({ id: store.id, name: store.name, price: store.price, }); const results = this.connection.save(storeEntity); return StoreRepository.toModel(results);}public async list() { const results = await this.connection.find(); return results.map((entity) =&gt; StoreRepository.toModel(entity));}public async get(id: string) { const result = await this.connection.findOneBy({ id, }); if(!result) { return undefined; } return StoreRepository.toModel(result);}public async update(store: Store) { await this.connection.update({id: store.id, },{name: store.name, price: store.price, });}public async delete(id: string) { const result = await this.connection.delete({ id,}); return result.affected ?? 0; }public static toModel(entity: StoreEntity | null): Store { return Store.create(entity);} } //Corrigir imports e adicionar outros métodos de acordo com o projeto</v>
       </c>
-      <c r="B12" s="72" t="str">
+      <c r="B12" s="59" t="str">
         <f>"&lt;-- Colar dentro de um arquivo .ts - nome sugerido: "&amp;LOWER(Entry!$I$1)&amp;".repository.ts"</f>
         <v>&lt;-- Colar dentro de um arquivo .ts - nome sugerido: store.repository.ts</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="76"/>
-      <c r="B13" s="77"/>
+      <c r="A13" s="63"/>
+      <c r="B13" s="64"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="69" t="s">
+      <c r="A14" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="73"/>
+      <c r="B14" s="60"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="70" t="str">
+      <c r="A15" s="57" t="str">
         <f>Engine!AA1&amp;Engine!Y2&amp;Engine!Y3&amp;Engine!Y4&amp;Engine!Y5&amp;Engine!Y6&amp;Engine!Y7&amp;Engine!Y8&amp;"} // Necessário configurar os validators e adicionar rotas de acordo com o projeto"</f>
         <v>import { Router } from 'express'; export const storeRoutes = () =&gt; { const app = Router(); app.get('/', new StoreController().list);app.get('/:id', new StoreController().get);app.post('/', newStoreController().create);app.put('/:id' ,new StoreController().update);app.delete('/:id' , newStoreController().delete);return app;} // Necessário configurar os validators e adicionar rotas de acordo com o projeto</v>
       </c>
-      <c r="B15" s="72" t="str">
+      <c r="B15" s="59" t="str">
         <f>"&lt;-- Colar dentro de um arquivo .ts - nome sugerido: "&amp;LOWER(Entry!$I$1)&amp;".routes.ts"</f>
         <v>&lt;-- Colar dentro de um arquivo .ts - nome sugerido: store.routes.ts</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="78"/>
-      <c r="B16" s="79"/>
+      <c r="A16" s="65"/>
+      <c r="B16" s="66"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>